<commit_message>
Fixed IRA eligibility assessment, wind and solar capex, some other small things
</commit_message>
<xml_diff>
--- a/src/ereznic2/H2_Analysis/green_steel_site_renewable_costs_ATB_aug2023.xlsx
+++ b/src/ereznic2/H2_Analysis/green_steel_site_renewable_costs_ATB_aug2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ereznic2\Documents\Projects\Wind-H2-Steel\Modeling\GreenSteel\src\ereznic2\H2_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFED6038-D76C-43EE-885E-BA3D172BC787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C423A22-BF73-450C-A1C3-90FB3B1AF2AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14700" yWindow="-1020" windowWidth="11988" windowHeight="13356" xr2:uid="{6F370ACC-2FEA-4034-9DAD-6260C657696D}"/>
+    <workbookView xWindow="-17388" yWindow="-4752" windowWidth="17496" windowHeight="30936" xr2:uid="{6F370ACC-2FEA-4034-9DAD-6260C657696D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -640,7 +640,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -817,19 +817,19 @@
         <v>49</v>
       </c>
       <c r="B9" s="4">
-        <v>1363</v>
+        <v>1302</v>
       </c>
       <c r="C9" s="4">
-        <v>1363</v>
+        <v>1302</v>
       </c>
       <c r="D9" s="6">
-        <v>1489</v>
+        <v>1422</v>
       </c>
       <c r="E9" s="4">
-        <v>1961</v>
+        <v>1873</v>
       </c>
       <c r="F9" s="4">
-        <v>1363</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -837,19 +837,19 @@
         <v>23</v>
       </c>
       <c r="B10" s="4">
-        <v>1268</v>
+        <v>1211</v>
       </c>
       <c r="C10" s="4">
-        <v>1268</v>
+        <v>1211</v>
       </c>
       <c r="D10" s="6">
-        <v>1362</v>
+        <v>1301</v>
       </c>
       <c r="E10" s="4">
-        <v>1772</v>
+        <v>1692</v>
       </c>
       <c r="F10" s="4">
-        <v>1268</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -857,19 +857,19 @@
         <v>24</v>
       </c>
       <c r="B11" s="4">
+        <v>1098</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1098</v>
+      </c>
+      <c r="D11" s="1">
         <v>1150</v>
       </c>
-      <c r="C11" s="4">
-        <v>1150</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1204</v>
-      </c>
       <c r="E11" s="4">
-        <v>1536</v>
+        <v>1467</v>
       </c>
       <c r="F11" s="4">
-        <v>1150</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -877,19 +877,19 @@
         <v>25</v>
       </c>
       <c r="B12" s="4">
+        <v>1044</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1044</v>
+      </c>
+      <c r="D12" s="1">
         <v>1093</v>
       </c>
-      <c r="C12" s="4">
-        <v>1093</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1145</v>
-      </c>
       <c r="E12" s="4">
-        <v>1462</v>
+        <v>1396</v>
       </c>
       <c r="F12" s="4">
-        <v>1093</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -897,19 +897,19 @@
         <v>26</v>
       </c>
       <c r="B13" s="4">
+        <v>882</v>
+      </c>
+      <c r="C13" s="4">
+        <v>882</v>
+      </c>
+      <c r="D13" s="1">
         <v>924</v>
       </c>
-      <c r="C13" s="4">
-        <v>924</v>
-      </c>
-      <c r="D13" s="1">
-        <v>968</v>
-      </c>
       <c r="E13" s="4">
-        <v>1241</v>
+        <v>1185</v>
       </c>
       <c r="F13" s="4">
-        <v>924</v>
+        <v>882</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -937,19 +937,19 @@
         <v>50</v>
       </c>
       <c r="B15" s="4">
-        <v>30.3</v>
+        <v>28.9</v>
       </c>
       <c r="C15" s="4">
-        <v>30.3</v>
+        <v>28.9</v>
       </c>
       <c r="D15" s="1">
-        <v>28.5</v>
+        <v>27.2</v>
       </c>
       <c r="E15" s="4">
-        <v>30.3</v>
+        <v>28.9</v>
       </c>
       <c r="F15" s="4">
-        <v>30.3</v>
+        <v>28.9</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -957,19 +957,19 @@
         <v>28</v>
       </c>
       <c r="B16" s="4">
-        <v>28.8</v>
+        <v>27.5</v>
       </c>
       <c r="C16" s="4">
-        <v>28.8</v>
+        <v>27.5</v>
       </c>
       <c r="D16" s="1">
-        <v>26.8</v>
+        <v>25.6</v>
       </c>
       <c r="E16" s="4">
-        <v>28.8</v>
+        <v>27.5</v>
       </c>
       <c r="F16" s="4">
-        <v>28.8</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -977,19 +977,19 @@
         <v>29</v>
       </c>
       <c r="B17" s="4">
-        <v>27</v>
+        <v>25.8</v>
       </c>
       <c r="C17" s="4">
-        <v>27</v>
+        <v>25.8</v>
       </c>
       <c r="D17" s="1">
-        <v>24.6</v>
+        <v>23.5</v>
       </c>
       <c r="E17" s="4">
-        <v>27</v>
+        <v>25.8</v>
       </c>
       <c r="F17" s="4">
-        <v>27</v>
+        <v>25.8</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -997,19 +997,19 @@
         <v>30</v>
       </c>
       <c r="B18" s="4">
-        <v>26.1</v>
+        <v>24.9</v>
       </c>
       <c r="C18" s="4">
-        <v>26.1</v>
+        <v>24.9</v>
       </c>
       <c r="D18" s="1">
-        <v>23.8</v>
+        <v>22.7</v>
       </c>
       <c r="E18" s="4">
-        <v>26.1</v>
+        <v>24.9</v>
       </c>
       <c r="F18" s="4">
-        <v>26.1</v>
+        <v>24.9</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1017,19 +1017,19 @@
         <v>31</v>
       </c>
       <c r="B19" s="4">
-        <v>23.3</v>
+        <v>22.3</v>
       </c>
       <c r="C19" s="4">
-        <v>23.3</v>
+        <v>22.3</v>
       </c>
       <c r="D19" s="1">
-        <v>21.3</v>
+        <v>20.3</v>
       </c>
       <c r="E19" s="4">
-        <v>23.3</v>
+        <v>22.3</v>
       </c>
       <c r="F19" s="4">
-        <v>23.3</v>
+        <v>22.3</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1065,19 +1065,19 @@
         <v>51</v>
       </c>
       <c r="B22" s="4">
-        <v>1291</v>
+        <v>1233</v>
       </c>
       <c r="C22" s="4">
-        <v>1291</v>
+        <v>1233</v>
       </c>
       <c r="D22" s="4">
-        <v>1291</v>
+        <v>1233</v>
       </c>
       <c r="E22" s="4">
-        <v>1291</v>
+        <v>1233</v>
       </c>
       <c r="F22" s="4">
-        <v>1291</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1085,19 +1085,19 @@
         <v>33</v>
       </c>
       <c r="B23" s="4">
-        <v>1248</v>
+        <v>1192</v>
       </c>
       <c r="C23" s="4">
-        <v>1248</v>
+        <v>1192</v>
       </c>
       <c r="D23" s="4">
-        <v>1248</v>
+        <v>1192</v>
       </c>
       <c r="E23" s="4">
-        <v>1248</v>
+        <v>1192</v>
       </c>
       <c r="F23" s="4">
-        <v>1248</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1105,19 +1105,19 @@
         <v>34</v>
       </c>
       <c r="B24" s="4">
-        <v>1038</v>
+        <v>991</v>
       </c>
       <c r="C24" s="4">
-        <v>1038</v>
+        <v>991</v>
       </c>
       <c r="D24" s="4">
-        <v>1038</v>
+        <v>991</v>
       </c>
       <c r="E24" s="4">
-        <v>1038</v>
+        <v>991</v>
       </c>
       <c r="F24" s="4">
-        <v>1038</v>
+        <v>991</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1125,19 +1125,19 @@
         <v>35</v>
       </c>
       <c r="B25" s="4">
-        <v>829</v>
+        <v>792</v>
       </c>
       <c r="C25" s="4">
-        <v>829</v>
+        <v>792</v>
       </c>
       <c r="D25" s="4">
-        <v>829</v>
+        <v>792</v>
       </c>
       <c r="E25" s="4">
-        <v>829</v>
+        <v>792</v>
       </c>
       <c r="F25" s="4">
-        <v>829</v>
+        <v>792</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1145,19 +1145,19 @@
         <v>36</v>
       </c>
       <c r="B26" s="4">
-        <v>632</v>
+        <v>604</v>
       </c>
       <c r="C26" s="4">
-        <v>632</v>
+        <v>604</v>
       </c>
       <c r="D26" s="4">
-        <v>632</v>
+        <v>604</v>
       </c>
       <c r="E26" s="4">
-        <v>632</v>
+        <v>604</v>
       </c>
       <c r="F26" s="4">
-        <v>632</v>
+        <v>604</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1185,19 +1185,19 @@
         <v>52</v>
       </c>
       <c r="B28" s="4">
-        <v>22.5</v>
+        <v>21.5</v>
       </c>
       <c r="C28" s="4">
-        <v>22.5</v>
+        <v>21.5</v>
       </c>
       <c r="D28" s="4">
-        <v>22.5</v>
+        <v>21.5</v>
       </c>
       <c r="E28" s="4">
-        <v>22.5</v>
+        <v>21.5</v>
       </c>
       <c r="F28" s="4">
-        <v>22.5</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1205,19 +1205,19 @@
         <v>38</v>
       </c>
       <c r="B29" s="4">
-        <v>20.5</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="C29" s="4">
-        <v>20.5</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="D29" s="4">
-        <v>20.5</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="E29" s="4">
-        <v>20.5</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="F29" s="4">
-        <v>20.5</v>
+        <v>19.600000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1225,19 +1225,19 @@
         <v>39</v>
       </c>
       <c r="B30" s="4">
-        <v>18</v>
+        <v>17.2</v>
       </c>
       <c r="C30" s="4">
-        <v>18</v>
+        <v>17.2</v>
       </c>
       <c r="D30" s="4">
-        <v>18</v>
+        <v>17.2</v>
       </c>
       <c r="E30" s="4">
-        <v>18</v>
+        <v>17.2</v>
       </c>
       <c r="F30" s="4">
-        <v>18</v>
+        <v>17.2</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1245,19 +1245,19 @@
         <v>40</v>
       </c>
       <c r="B31" s="4">
-        <v>15.5</v>
+        <v>14.8</v>
       </c>
       <c r="C31" s="4">
-        <v>15.5</v>
+        <v>14.8</v>
       </c>
       <c r="D31" s="4">
-        <v>15.5</v>
+        <v>14.8</v>
       </c>
       <c r="E31" s="4">
-        <v>15.5</v>
+        <v>14.8</v>
       </c>
       <c r="F31" s="4">
-        <v>15.5</v>
+        <v>14.8</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1265,19 +1265,19 @@
         <v>41</v>
       </c>
       <c r="B32" s="4">
-        <v>13.5</v>
+        <v>12.9</v>
       </c>
       <c r="C32" s="4">
-        <v>13.5</v>
+        <v>12.9</v>
       </c>
       <c r="D32" s="4">
-        <v>13.5</v>
+        <v>12.9</v>
       </c>
       <c r="E32" s="4">
-        <v>13.5</v>
+        <v>12.9</v>
       </c>
       <c r="F32" s="4">
-        <v>13.5</v>
+        <v>12.9</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated code to enable full wind-only to solar-only sweep
</commit_message>
<xml_diff>
--- a/src/ereznic2/H2_Analysis/green_steel_site_renewable_costs_ATB_aug2023.xlsx
+++ b/src/ereznic2/H2_Analysis/green_steel_site_renewable_costs_ATB_aug2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ereznic2\Documents\Projects\Wind-H2-Steel\Modeling\GreenSteel\src\ereznic2\H2_Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evan\Documents\Work\Green steel\Modeling\GreenSteel\src\ereznic2\H2_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C423A22-BF73-450C-A1C3-90FB3B1AF2AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1C6F3F-E7A6-40CD-9F14-6D34C332DF56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17388" yWindow="-4752" windowWidth="17496" windowHeight="30936" xr2:uid="{6F370ACC-2FEA-4034-9DAD-6260C657696D}"/>
+    <workbookView xWindow="5160" yWindow="1695" windowWidth="16695" windowHeight="19470" xr2:uid="{6F370ACC-2FEA-4034-9DAD-6260C657696D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -341,9 +341,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -381,7 +381,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -487,7 +487,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -629,7 +629,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -640,19 +640,19 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="F3" sqref="F3:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -672,7 +672,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -692,7 +692,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -712,7 +712,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -732,7 +732,7 @@
         <v>47.523299999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -752,7 +752,7 @@
         <v>-92.536600000000007</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -772,7 +772,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -792,7 +792,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -812,7 +812,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>49</v>
       </c>
@@ -832,7 +832,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
@@ -852,7 +852,7 @@
         <v>1211</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
@@ -872,7 +872,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
@@ -892,7 +892,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
@@ -912,7 +912,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
@@ -932,7 +932,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>50</v>
       </c>
@@ -952,7 +952,7 @@
         <v>28.9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>28</v>
       </c>
@@ -972,7 +972,7 @@
         <v>27.5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
@@ -992,7 +992,7 @@
         <v>25.8</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>30</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>24.9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>31</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>22.3</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>6.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1060,7 +1060,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>51</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>33</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>1192</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>34</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>35</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>37</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>52</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>38</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>39</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>40</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>41</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>42</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>5.8000000000000003E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1308,7 +1308,7 @@
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>43</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>44</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>45</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>46</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>22.1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>47</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>46.97</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>48</v>
       </c>
@@ -1439,7 +1439,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1451,7 +1451,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Initial updates to correct wind and solar capacity factors
</commit_message>
<xml_diff>
--- a/src/ereznic2/H2_Analysis/green_steel_site_renewable_costs_ATB_aug2023.xlsx
+++ b/src/ereznic2/H2_Analysis/green_steel_site_renewable_costs_ATB_aug2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evan\Documents\Work\Green steel\Modeling\GreenSteel\src\ereznic2\H2_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1C6F3F-E7A6-40CD-9F14-6D34C332DF56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8882843-C4EA-4FCA-B6A0-14E805661994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5160" yWindow="1695" windowWidth="16695" windowHeight="19470" xr2:uid="{6F370ACC-2FEA-4034-9DAD-6260C657696D}"/>
+    <workbookView xWindow="7275" yWindow="1320" windowWidth="38700" windowHeight="15885" xr2:uid="{6F370ACC-2FEA-4034-9DAD-6260C657696D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -82,9 +82,6 @@
     <t>41.62, -87.22</t>
   </si>
   <si>
-    <t>34.22, -102.75</t>
-  </si>
-  <si>
     <t>42.55, -90.69</t>
   </si>
   <si>
@@ -241,6 +238,9 @@
       </rPr>
       <t xml:space="preserve"> PV OpEx</t>
     </r>
+  </si>
+  <si>
+    <t>34.223, -102.245</t>
   </si>
 </sst>
 </file>
@@ -640,7 +640,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,27 +700,27 @@
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1">
         <v>41.62</v>
       </c>
       <c r="C4" s="1">
-        <v>34.22</v>
+        <v>34.334000000000003</v>
       </c>
       <c r="D4" s="1">
         <v>42.55</v>
@@ -734,13 +734,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1">
         <v>-87.22</v>
       </c>
       <c r="C5" s="1">
-        <v>-102.75</v>
+        <v>-102.245</v>
       </c>
       <c r="D5" s="1">
         <v>-90.69</v>
@@ -754,7 +754,7 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="4">
         <v>6</v>
@@ -774,7 +774,7 @@
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="4">
         <v>170</v>
@@ -794,7 +794,7 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="4">
         <v>115</v>
@@ -814,7 +814,7 @@
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="4">
         <v>1302</v>
@@ -834,7 +834,7 @@
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="4">
         <v>1211</v>
@@ -854,7 +854,7 @@
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="4">
         <v>1098</v>
@@ -874,7 +874,7 @@
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="4">
         <v>1044</v>
@@ -894,7 +894,7 @@
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="4">
         <v>882</v>
@@ -914,7 +914,7 @@
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="4">
         <v>1.1000000000000001</v>
@@ -934,7 +934,7 @@
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" s="4">
         <v>28.9</v>
@@ -954,7 +954,7 @@
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="4">
         <v>27.5</v>
@@ -974,7 +974,7 @@
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="4">
         <v>25.8</v>
@@ -994,7 +994,7 @@
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="4">
         <v>24.9</v>
@@ -1014,7 +1014,7 @@
     </row>
     <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="4">
         <v>22.3</v>
@@ -1034,7 +1034,7 @@
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="4">
         <v>6.0999999999999999E-2</v>
@@ -1062,7 +1062,7 @@
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" s="4">
         <v>1233</v>
@@ -1082,7 +1082,7 @@
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" s="4">
         <v>1192</v>
@@ -1102,7 +1102,7 @@
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" s="4">
         <v>991</v>
@@ -1122,7 +1122,7 @@
     </row>
     <row r="25" spans="1:6" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" s="4">
         <v>792</v>
@@ -1142,7 +1142,7 @@
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B26" s="4">
         <v>604</v>
@@ -1162,7 +1162,7 @@
     </row>
     <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" s="1">
         <v>1</v>
@@ -1182,7 +1182,7 @@
     </row>
     <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" s="4">
         <v>21.5</v>
@@ -1202,7 +1202,7 @@
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="4">
         <v>19.600000000000001</v>
@@ -1222,7 +1222,7 @@
     </row>
     <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" s="4">
         <v>17.2</v>
@@ -1242,7 +1242,7 @@
     </row>
     <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" s="4">
         <v>14.8</v>
@@ -1262,7 +1262,7 @@
     </row>
     <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" s="4">
         <v>12.9</v>
@@ -1282,7 +1282,7 @@
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" s="4">
         <v>5.8000000000000003E-2</v>
@@ -1310,7 +1310,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B35" s="1">
         <v>100</v>
@@ -1330,7 +1330,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B36" s="1">
         <v>190</v>
@@ -1350,7 +1350,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B37" s="1">
         <v>207</v>
@@ -1370,7 +1370,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B38" s="1">
         <v>15.3</v>
@@ -1390,7 +1390,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B39" s="1">
         <v>27.89</v>
@@ -1410,7 +1410,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B40" s="1">
         <v>14.52</v>

</xml_diff>

<commit_message>
Updated script to correctly handle AC/DC solar nomenclature
</commit_message>
<xml_diff>
--- a/src/ereznic2/H2_Analysis/green_steel_site_renewable_costs_ATB_aug2023.xlsx
+++ b/src/ereznic2/H2_Analysis/green_steel_site_renewable_costs_ATB_aug2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evan\Documents\Work\Green steel\Modeling\GreenSteel\src\ereznic2\H2_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8882843-C4EA-4FCA-B6A0-14E805661994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0381E0D-067E-45A1-BEE7-75CD21F1D3DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7275" yWindow="1320" windowWidth="38700" windowHeight="15885" xr2:uid="{6F370ACC-2FEA-4034-9DAD-6260C657696D}"/>
+    <workbookView xWindow="4425" yWindow="2010" windowWidth="38700" windowHeight="15885" xr2:uid="{6F370ACC-2FEA-4034-9DAD-6260C657696D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -82,13 +82,7 @@
     <t>41.62, -87.22</t>
   </si>
   <si>
-    <t>42.55, -90.69</t>
-  </si>
-  <si>
     <t>30.45, -89.35</t>
-  </si>
-  <si>
-    <t>47.5233, -92.5366</t>
   </si>
   <si>
     <t>Lat</t>
@@ -241,6 +235,12 @@
   </si>
   <si>
     <t>34.223, -102.245</t>
+  </si>
+  <si>
+    <t>42.4, -90.85</t>
+  </si>
+  <si>
+    <t>47.5, -92.55</t>
   </si>
 </sst>
 </file>
@@ -640,7 +640,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,21 +700,21 @@
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1">
         <v>41.62</v>
@@ -723,18 +723,18 @@
         <v>34.334000000000003</v>
       </c>
       <c r="D4" s="1">
-        <v>42.55</v>
+        <v>42.4</v>
       </c>
       <c r="E4" s="1">
         <v>30.45</v>
       </c>
       <c r="F4" s="1">
-        <v>47.523299999999999</v>
+        <v>47.5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1">
         <v>-87.22</v>
@@ -743,18 +743,18 @@
         <v>-102.245</v>
       </c>
       <c r="D5" s="1">
-        <v>-90.69</v>
+        <v>-90.85</v>
       </c>
       <c r="E5" s="1">
         <v>-89.35</v>
       </c>
       <c r="F5" s="1">
-        <v>-92.536600000000007</v>
+        <v>-92.55</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" s="4">
         <v>6</v>
@@ -774,7 +774,7 @@
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="4">
         <v>170</v>
@@ -794,7 +794,7 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" s="4">
         <v>115</v>
@@ -814,7 +814,7 @@
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" s="4">
         <v>1302</v>
@@ -834,7 +834,7 @@
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B10" s="4">
         <v>1211</v>
@@ -854,7 +854,7 @@
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B11" s="4">
         <v>1098</v>
@@ -874,7 +874,7 @@
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12" s="4">
         <v>1044</v>
@@ -894,7 +894,7 @@
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B13" s="4">
         <v>882</v>
@@ -914,7 +914,7 @@
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" s="4">
         <v>1.1000000000000001</v>
@@ -934,7 +934,7 @@
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B15" s="4">
         <v>28.9</v>
@@ -954,7 +954,7 @@
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B16" s="4">
         <v>27.5</v>
@@ -974,7 +974,7 @@
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B17" s="4">
         <v>25.8</v>
@@ -994,7 +994,7 @@
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B18" s="4">
         <v>24.9</v>
@@ -1014,7 +1014,7 @@
     </row>
     <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B19" s="4">
         <v>22.3</v>
@@ -1034,7 +1034,7 @@
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B20" s="4">
         <v>6.0999999999999999E-2</v>
@@ -1062,7 +1062,7 @@
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B22" s="4">
         <v>1233</v>
@@ -1082,7 +1082,7 @@
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B23" s="4">
         <v>1192</v>
@@ -1102,7 +1102,7 @@
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B24" s="4">
         <v>991</v>
@@ -1122,7 +1122,7 @@
     </row>
     <row r="25" spans="1:6" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B25" s="4">
         <v>792</v>
@@ -1142,7 +1142,7 @@
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B26" s="4">
         <v>604</v>
@@ -1162,7 +1162,7 @@
     </row>
     <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B27" s="1">
         <v>1</v>
@@ -1182,7 +1182,7 @@
     </row>
     <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B28" s="4">
         <v>21.5</v>
@@ -1202,7 +1202,7 @@
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B29" s="4">
         <v>19.600000000000001</v>
@@ -1222,7 +1222,7 @@
     </row>
     <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B30" s="4">
         <v>17.2</v>
@@ -1242,7 +1242,7 @@
     </row>
     <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B31" s="4">
         <v>14.8</v>
@@ -1262,7 +1262,7 @@
     </row>
     <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B32" s="4">
         <v>12.9</v>
@@ -1282,7 +1282,7 @@
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B33" s="4">
         <v>5.8000000000000003E-2</v>
@@ -1310,7 +1310,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B35" s="1">
         <v>100</v>
@@ -1330,7 +1330,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B36" s="1">
         <v>190</v>
@@ -1350,7 +1350,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B37" s="1">
         <v>207</v>
@@ -1370,7 +1370,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B38" s="1">
         <v>15.3</v>
@@ -1390,7 +1390,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B39" s="1">
         <v>27.89</v>
@@ -1410,7 +1410,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B40" s="1">
         <v>14.52</v>

</xml_diff>